<commit_message>
clean up; reduce option value len
</commit_message>
<xml_diff>
--- a/apps/pc_zone/test/support/data/shopee-simple-built-variants.xlsx
+++ b/apps/pc_zone/test/support/data/shopee-simple-built-variants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achilles/Projects/pczone_umbrella/apps/pc_zone/test/support/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D51EE5A-EBFF-D940-81B8-83504BFDCF1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD42738C-B7CA-2E4D-B302-5E0978B9CC05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,18 +46,6 @@
     <t>Hp Elitedesk 800 G2 Mini</t>
   </si>
   <si>
-    <t>i5-6500T, Không RAM + Không ổ cứng</t>
-  </si>
-  <si>
-    <t>i5-6500T, Không RAM + 256GB NVMe 95%</t>
-  </si>
-  <si>
-    <t>i5-6500T, Không RAM + 256GB NVMe</t>
-  </si>
-  <si>
-    <t>i5-6500T, Không RAM + 512GB NVMe</t>
-  </si>
-  <si>
     <t>aaa</t>
   </si>
   <si>
@@ -71,16 +59,33 @@
   </si>
   <si>
     <t>x4</t>
+  </si>
+  <si>
+    <t>i5-6500T; Không RAM, 256GB NVMe 95%</t>
+  </si>
+  <si>
+    <t>i5-6500T; Không RAM, 256GB NVMe</t>
+  </si>
+  <si>
+    <t>i5-6500;, Không RAM, 512GB NVMe</t>
+  </si>
+  <si>
+    <t>i5-6500T; Không RAM, Không SSD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,7 +428,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -467,13 +473,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F2">
         <v>3500000</v>
@@ -490,13 +496,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F3">
         <v>4250000</v>
@@ -513,13 +519,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="F4">
         <v>4300000</v>
@@ -536,13 +542,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F5">
         <v>4800000</v>

</xml_diff>